<commit_message>
AR code for updated performer changes for UAT
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grmusarpadev11\Desktop\grm-usa-ar-sap-ariba\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grmusarpadev11\Desktop\AT_Performer\grm-usa-ar-ariba-performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104E2E81-1CF3-489D-A132-C06ED4B9C55E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007F3E80-5715-4322-A292-0AB0BC5AA2BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -267,6 +267,77 @@
   </si>
   <si>
     <t>Mars</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_SharePointCredential</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_ApplicationSecret</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_TenantID</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_ApplicationID</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_AGENCYNAME_Target_Performer</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_CLIENTNAME_Target_Performer</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_DriveName_Target</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_SiteUrl_Target</t>
+  </si>
+  <si>
+    <t>ProfileDirectory</t>
+  </si>
+  <si>
+    <t>C:\1files\chrome-profiles\bot</t>
+  </si>
+  <si>
+    <t>C:\Program Files\Google\Chrome\Application\chrome.exe</t>
+  </si>
+  <si>
+    <t>ChromeExtension_Path</t>
+  </si>
+  <si>
+    <t>Order Status was not New or Partial</t>
+  </si>
+  <si>
+    <t>BEXS0003</t>
+  </si>
+  <si>
+    <t>Email_To</t>
+  </si>
+  <si>
+    <t>Email_CC</t>
+  </si>
+  <si>
+    <t>Email_Subject</t>
+  </si>
+  <si>
+    <t>Email_Body</t>
+  </si>
+  <si>
+    <t>GM-USA_AR Execution Report</t>
+  </si>
+  <si>
+    <t>&lt;body&gt;&lt;p&gt;Hi Team,&lt;br/&gt;
+All invoices are processed for SAP Ariba, 
+Please Find Below file path for your reference.
+&lt;br/&gt;&lt;a href={0}&gt;USA_AR_TARGETREPORT &lt;/a&gt;&lt;br/&gt;&lt;br/&gt;&lt;p&gt;&lt;/body&gt;&lt;br/&gt;
+Thanks, &lt;br/&gt;
+RPA Robot.</t>
+  </si>
+  <si>
+    <t>gajanan.patil@accelirate.com</t>
+  </si>
+  <si>
+    <t>-3</t>
   </si>
 </sst>
 </file>
@@ -284,6 +355,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -351,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -375,6 +447,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,7 +767,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -780,8 +855,8 @@
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B8">
-        <v>3</v>
+      <c r="B8" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>59</v>
@@ -840,10 +915,30 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1836,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1970,10 +2065,38 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -2957,13 +3080,12 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="1" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
@@ -3058,13 +3180,62 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -4059,7 +4230,7 @@
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4230,6 +4401,14 @@
         <v>68</v>
       </c>
     </row>
+    <row r="5" spans="1:26">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="6" spans="1:26">
       <c r="A6" s="2"/>
     </row>

</xml_diff>

<commit_message>
Split out Mars as separate performer
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grmusarpadev11\Documents\grm-usa-ar-ariba-Performer\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8AE8E3-BC1D-4E57-BAB1-F54A561110F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C9FDB-9351-4A38-9BB1-612C204C708C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -293,21 +293,12 @@
     <t>BEXS0003</t>
   </si>
   <si>
-    <t>Email_To</t>
-  </si>
-  <si>
-    <t>Email_CC</t>
-  </si>
-  <si>
     <t>Email_Subject</t>
   </si>
   <si>
     <t>Email_Body</t>
   </si>
   <si>
-    <t>tom.kelshaw@wmglobal.com</t>
-  </si>
-  <si>
     <t>EXS0008</t>
   </si>
   <si>
@@ -315,12 +306,6 @@
   </si>
   <si>
     <t>Mars_PDF_FilePath</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>anita.kapur@accelirate.com</t>
   </si>
   <si>
     <t>GM_USA_AR Status Report</t>
@@ -425,9 +410,6 @@
 RPA Robot.</t>
   </si>
   <si>
-    <t>-96</t>
-  </si>
-  <si>
     <t>BEXS0004</t>
   </si>
   <si>
@@ -445,16 +427,34 @@
 The Below info is for tech support team to analyize the issue</t>
   </si>
   <si>
-    <t>gajanan.patil@accelirate.com</t>
-  </si>
-  <si>
     <t>Bill Amount is negative but Devision is not Corporate for Shell.</t>
   </si>
   <si>
     <t>BEXS0005</t>
   </si>
   <si>
-    <t>kumar.bhawan@accelirate.com</t>
+    <t>GMUSA_AR_EmailCC</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_Performer_Mail_CC</t>
+  </si>
+  <si>
+    <t>Mars_Queue_Name</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_EmailBcc</t>
+  </si>
+  <si>
+    <t>GMUSA_AR_Performer_Mail_BCC</t>
+  </si>
+  <si>
+    <t>Sharepoint Login Creds</t>
+  </si>
+  <si>
+    <t>-36</t>
+  </si>
+  <si>
+    <t>GMUSAAR_MARS</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="###,000"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -631,6 +631,11 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF4E5E65"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="22">
@@ -1011,7 +1016,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1025,12 +1029,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="59">
     <cellStyle name="Comma 2" xfId="38" xr:uid="{B0A0F9FC-9ADB-4FDF-AD5C-0A7345AEB1BA}"/>
@@ -1403,18 +1408,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="8" customFormat="1" ht="14.25" customHeight="1">
@@ -1462,7 +1467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="28.8">
+    <row r="3" spans="1:26" ht="29">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1494,8 +1499,8 @@
       <c r="A8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>129</v>
+      <c r="B8" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>57</v>
@@ -1525,19 +1530,19 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
         <v>95</v>
-      </c>
-      <c r="B11" t="s">
-        <v>100</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -1562,18 +1567,18 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>67</v>
@@ -1589,27 +1594,33 @@
       <c r="B17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="17" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+    <row r="20" spans="1:3" s="25" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A20" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2590,7 +2601,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2602,16 +2612,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="65.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="65.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2648,7 +2658,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2665,7 +2675,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -2740,76 +2750,53 @@
       <c r="A13" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>92</v>
-      </c>
+      <c r="B13" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="19"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="15"/>
+      <c r="B14" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>97</v>
-      </c>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="16.8" customHeight="1">
-      <c r="B17" s="4"/>
-      <c r="C17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.899999999999999" customHeight="1">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -3768,13 +3755,8 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
-  <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" xr:uid="{171D987C-ECDA-48E2-B05E-15A150050EE0}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{4B19CD85-1219-49D7-8B8F-DB99CC3C2101}"/>
-    <hyperlink ref="B13" r:id="rId3" xr:uid="{4171441C-6A9F-4F38-9E32-79CEEB4FCD9A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3782,15 +3764,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="2" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3880,7 +3862,7 @@
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3911,22 +3893,22 @@
       <c r="A11" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>111</v>
+      <c r="B11" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>118</v>
+      <c r="B12" s="21" t="s">
+        <v>113</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -3934,10 +3916,10 @@
         <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -3945,136 +3927,150 @@
         <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>112</v>
+        <v>109</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A17" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A18" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A17" s="24" t="s">
+      <c r="E18" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A19" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A20" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A21" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A22" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B22" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A18" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A19" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A20" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A21" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A22" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>105</v>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:5" ht="14.25" customHeight="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A25" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A26" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:5" ht="14.25" customHeight="1"/>
@@ -5055,15 +5051,15 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" style="13" customWidth="1"/>
     <col min="2" max="2" width="98" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="13"/>
+    <col min="4" max="16384" width="9.1796875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="12" customFormat="1" ht="14.25" customHeight="1">
@@ -5116,20 +5112,20 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="28.8">
+      <c r="B5" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="29">
       <c r="A6" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>134</v>
+      <c r="B6" s="24" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -5158,18 +5154,18 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="14" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -5185,9 +5181,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" customWidth="1"/>
     <col min="2" max="2" width="98" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
   </cols>
@@ -5247,23 +5243,23 @@
         <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26">
-      <c r="A7" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>136</v>
+      <c r="B7" s="26" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:26">

</xml_diff>

<commit_message>
added Updated Repo for Shell and Target, removed Mars subprocess
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grmusarpadev11\Documents\grm-usa-ar-ariba-Performer\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C9FDB-9351-4A38-9BB1-612C204C708C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8AE8E3-BC1D-4E57-BAB1-F54A561110F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -293,12 +293,21 @@
     <t>BEXS0003</t>
   </si>
   <si>
+    <t>Email_To</t>
+  </si>
+  <si>
+    <t>Email_CC</t>
+  </si>
+  <si>
     <t>Email_Subject</t>
   </si>
   <si>
     <t>Email_Body</t>
   </si>
   <si>
+    <t>tom.kelshaw@wmglobal.com</t>
+  </si>
+  <si>
     <t>EXS0008</t>
   </si>
   <si>
@@ -306,6 +315,12 @@
   </si>
   <si>
     <t>Mars_PDF_FilePath</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>anita.kapur@accelirate.com</t>
   </si>
   <si>
     <t>GM_USA_AR Status Report</t>
@@ -410,6 +425,9 @@
 RPA Robot.</t>
   </si>
   <si>
+    <t>-96</t>
+  </si>
+  <si>
     <t>BEXS0004</t>
   </si>
   <si>
@@ -427,34 +445,16 @@
 The Below info is for tech support team to analyize the issue</t>
   </si>
   <si>
+    <t>gajanan.patil@accelirate.com</t>
+  </si>
+  <si>
     <t>Bill Amount is negative but Devision is not Corporate for Shell.</t>
   </si>
   <si>
     <t>BEXS0005</t>
   </si>
   <si>
-    <t>GMUSA_AR_EmailCC</t>
-  </si>
-  <si>
-    <t>GMUSA_AR_Performer_Mail_CC</t>
-  </si>
-  <si>
-    <t>Mars_Queue_Name</t>
-  </si>
-  <si>
-    <t>GMUSA_AR_EmailBcc</t>
-  </si>
-  <si>
-    <t>GMUSA_AR_Performer_Mail_BCC</t>
-  </si>
-  <si>
-    <t>Sharepoint Login Creds</t>
-  </si>
-  <si>
-    <t>-36</t>
-  </si>
-  <si>
-    <t>GMUSAAR_MARS</t>
+    <t>kumar.bhawan@accelirate.com</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="###,000"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -631,11 +631,6 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF4E5E65"/>
-      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="22">
@@ -1016,6 +1011,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1029,13 +1025,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="59">
     <cellStyle name="Comma 2" xfId="38" xr:uid="{B0A0F9FC-9ADB-4FDF-AD5C-0A7345AEB1BA}"/>
@@ -1408,18 +1403,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="8" customFormat="1" ht="14.25" customHeight="1">
@@ -1467,7 +1462,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="29">
+    <row r="3" spans="1:26" ht="28.8">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1499,8 +1494,8 @@
       <c r="A8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>137</v>
+      <c r="B8" s="17" t="s">
+        <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>57</v>
@@ -1530,19 +1525,19 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -1567,18 +1562,18 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>67</v>
@@ -1594,33 +1589,27 @@
       <c r="B17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>136</v>
-      </c>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="19" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="25" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A20" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>138</v>
-      </c>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2601,6 +2590,7 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2612,16 +2602,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="65.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2658,7 +2648,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2675,7 +2665,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -2750,53 +2740,76 @@
       <c r="A13" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="19"/>
+      <c r="B13" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>123</v>
-      </c>
+      <c r="B14" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B15" s="4"/>
+      <c r="A15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16.899999999999999" customHeight="1">
-      <c r="A17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+      <c r="A16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16.8" customHeight="1">
+      <c r="B17" s="4"/>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -3755,8 +3768,13 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
+  <hyperlinks>
+    <hyperlink ref="C15" r:id="rId1" xr:uid="{171D987C-ECDA-48E2-B05E-15A150050EE0}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{4B19CD85-1219-49D7-8B8F-DB99CC3C2101}"/>
+    <hyperlink ref="B13" r:id="rId3" xr:uid="{4171441C-6A9F-4F38-9E32-79CEEB4FCD9A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3764,15 +3782,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="2" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3862,7 +3880,7 @@
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3893,22 +3911,22 @@
       <c r="A11" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>106</v>
+      <c r="B11" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>113</v>
+      <c r="B12" s="22" t="s">
+        <v>118</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -3916,10 +3934,10 @@
         <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -3927,150 +3945,136 @@
         <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>107</v>
+        <v>114</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>108</v>
+        <v>115</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A17" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="22" t="s">
+      <c r="A17" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A19" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B19" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A19" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="22" t="s">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A20" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A21" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A22" s="24" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A20" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" s="22" t="s">
+      <c r="B22" s="24" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A21" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A22" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>100</v>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A25" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A26" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>135</v>
-      </c>
-    </row>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:5" ht="14.25" customHeight="1"/>
@@ -5051,15 +5055,15 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.7265625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="98" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="13"/>
+    <col min="4" max="16384" width="9.109375" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="12" customFormat="1" ht="14.25" customHeight="1">
@@ -5112,20 +5116,20 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="29">
+      <c r="B5" s="26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="28.8">
       <c r="A6" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>128</v>
+      <c r="B6" s="26" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -5154,18 +5158,18 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="13" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="14" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -5181,9 +5185,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.7265625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="98" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
   </cols>
@@ -5243,23 +5247,23 @@
         <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>129</v>
+      <c r="A7" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:26">

</xml_diff>